<commit_message>
changes from last days
</commit_message>
<xml_diff>
--- a/relecov_tools/example_data/dummy_data_small.xlsx
+++ b/relecov_tools/example_data/dummy_data_small.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t xml:space="preserve">Collecting Sample id</t>
   </si>
   <si>
-    <t xml:space="preserve">Collecting Institution</t>
+    <t xml:space="preserve">Originating Laboratory</t>
   </si>
   <si>
     <t xml:space="preserve">Submitting Institution</t>
@@ -34,75 +34,167 @@
     <t xml:space="preserve">Sample Collection Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Community</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isolate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Host Scientific Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Host Disease</t>
+    <t xml:space="preserve">geo_loc_country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geo_loc_state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">organism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isolate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">host_scientific_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Host Common Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">host_disease</t>
   </si>
   <si>
     <t xml:space="preserve">Sequencing Instrument Model</t>
   </si>
   <si>
-    <t xml:space="preserve">Sequencing Platforms </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consensus Sequence Software Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consensus Sequence Software Version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prov_rona_99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Navarra Biotech!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNM_1212_aaa</t>
+    <t xml:space="preserve">Sequencing Platforms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consensus_sequence_software_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consensus_sequence_software_version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample_description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library Selection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library Strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library Layout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GISAID Virus Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GISAID Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Originating Laboratory Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">broker_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nominal_sdev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first_created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospital Universitario de Basurto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laboratorio de Microbiología de Bibao </t>
   </si>
   <si>
     <t xml:space="preserve">Spain</t>
   </si>
   <si>
-    <t xml:space="preserve">e.g:Madrid</t>
+    <t xml:space="preserve">Madrid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Severe acute respiratory syndrome coronavirus 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARS-CoV-2/human/USA/CA-CDPH-001/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homo sapiens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARS-CoV2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Illumina MiSeq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILLUMINA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLC Genomics Workbench 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">. CLC Genomics Workbench 12,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filename2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">madnatory ENA description sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METAGENOMIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RANDOM PCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAIRED</t>
   </si>
   <si>
     <t xml:space="preserve">betacoronavirus</t>
   </si>
   <si>
-    <t xml:space="preserve">SARS-CoV-2/human/USA/CA-CDPH-001/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Human</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Illumina Miseq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ILLUMINA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLC Genomics Workbench 12</t>
+    <t xml:space="preserve">hCoV-19/España/Vizcaya-01/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GISAID-Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avda. Montevideo,18  BilbaoVizcaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P17157_1007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P17157_1008</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -176,7 +268,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -185,11 +277,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -210,15 +310,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S3" activeCellId="0" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="47.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -240,7 +343,7 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -260,48 +363,229 @@
       </c>
       <c r="N1" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="59.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>20</v>
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>44743</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>19</v>
+        <v>36</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="2" t="n">
+        <v>2697049</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB2" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AC2" s="5" t="n">
+        <v>44050</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="59.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>44743</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="2" t="n">
+        <v>2697049</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z3" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB3" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AC3" s="5" t="n">
+        <v>44050</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in schemas and validation module
</commit_message>
<xml_diff>
--- a/relecov_tools/example_data/dummy_data_small.xlsx
+++ b/relecov_tools/example_data/dummy_data_small.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="130">
   <si>
     <t xml:space="preserve">Collecting Sample id</t>
   </si>
@@ -109,6 +109,123 @@
     <t xml:space="preserve">first_created</t>
   </si>
   <si>
+    <t xml:space="preserve">sra_ftp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sra_aspera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sra_galaxy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sra_md5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sra_bytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">submitted_format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">submitted_galaxy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">submitted_aspera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">submitted_ftp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">submitted_md5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">submitted_bytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fastq_galaxy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fastq_aspera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fastq_ftp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fastq_md5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fastq_bytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_alias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">experiment_alias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">study_alias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">study_title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">experiment_title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">last_updated_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first_public_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">center_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">submission_accession</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_accession</t>
+  </si>
+  <si>
+    <t xml:space="preserve">experiment_accession</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secondary_sample_accession</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample_accession</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secondary_study_accession</t>
+  </si>
+  <si>
+    <t xml:space="preserve">study_accession</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read_length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">analysis_accession</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nominal_length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">library_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample_storage_conditions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">common_name</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID_001</t>
   </si>
   <si>
@@ -166,35 +283,144 @@
     <t xml:space="preserve">WGS</t>
   </si>
   <si>
+    <t xml:space="preserve">CTS strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">betacoronavirus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hCoV-19/España/Vizcaya-01/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GISAID-Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avda. Montevideo,18  BilbaoVizcaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P17157_1007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2cf0d467d6dc4ae0a5473774d54c059c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ftp.sra.ebi.ac.uk/vol1/err/ERR438/005/ERR4387385</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fasp.sra.ebi.ac.uk:/vol1/err/ERR438/005/ERR4387385</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FASTQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ftp.sra.ebi.ac.uk/vol1/run/ERR438/ERR4387385/P17157_1007_S7_L001_R1_001.fastq.gz;ftp.sra.ebi.ac.uk/vol1/run/ERR438/ERR4387385/P17157_1007_S7_L001_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fasp.sra.ebi.ac.uk:/vol1/run/ERR438/ERR4387385/P17157_1007_S7_L001_R1_001.fastq.gz;fasp.sra.ebi.ac.uk:/vol1/run/ERR438/ERR4387385/P17157_1007_S7_L001_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d726a9abc918e2b43bd68b24c7d01b3a;f01eba1b2bad974bdf61b81b1ae8ac2a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ftp.sra.ebi.ac.uk/vol1/fastq/ERR438/005/ERR4387385/ERR4387385_1.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fasp.sra.ebi.ac.uk:/vol1/fastq/ERR438/005/ERR4387385/ERR4387385_1.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ftp.sra.ebi.ac.uk/vol1/fastq/ERR438/005/ERR4387385/ERR4387385_1.fastq.gz;ftp.sra.ebi.ac.uk/vol1/fastq/ERR438/005/ERR4387385/ERR4387385_2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIDE_0000469</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS_1000568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ena-RUN-KAROLINSKA INSITUTET-29-07-2020-14:50:07:151-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ena-EXPERIMENT-KAROLINSKA INSITUTET-29-07-2020-14:50:07:151-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ena-STUDY-KAROLINSKA INSITUTET-29-07-2020-14:18:07:925-2092</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARS-CoV-2 genomes from late April in Stockholm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Illumina MiSeq paired end sequencing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-07-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-08-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KAROLINSKA INSITUTET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERA2794974</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERX4331406</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERS4858671</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMEA7098096</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERP123173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRJEB39632</t>
+  </si>
+  <si>
     <t xml:space="preserve">PAIRED</t>
   </si>
   <si>
-    <t xml:space="preserve">betacoronavirus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hCoV-19/España/Vizcaya-01/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GISAID-Username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avda. Montevideo,18  BilbaoVizcaya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P17157_1007</t>
+    <t xml:space="preserve">24 degrees celsius</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">P17157_1008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIDE_0000470</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ena-STUDY-KAROLINSKA INSITUTET-29-07-2020-14:18:07:925-2093</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-08-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERA2794975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERX4331407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SINGLE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -268,7 +494,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -293,6 +519,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -310,14 +540,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC3"/>
+  <dimension ref="A1:BP3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S3" activeCellId="0" sqref="S3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BG1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BP2" activeCellId="0" sqref="BP2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="0" width="23.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -409,88 +640,205 @@
       <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="AD1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="BO1" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" s="0" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="59.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="197.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>44743</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="Q2" s="2" t="n">
         <v>2697049</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="AB2" s="0" t="n">
         <v>0.1</v>
@@ -498,94 +846,313 @@
       <c r="AC2" s="5" t="n">
         <v>44050</v>
       </c>
+      <c r="AD2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AG2" s="2" t="n">
+        <v>260236789</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM2" s="2" t="n">
+        <v>139853010</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AY2" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="AZ2" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB2" s="2" t="n">
+        <v>503907110</v>
+      </c>
+      <c r="BC2" s="2" t="n">
+        <v>837055</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="BG2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="BH2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="BI2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="BM2" s="0" t="n">
+        <v>350</v>
+      </c>
+      <c r="BN2" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="BO2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="BP2" s="0" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="59.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="197.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>44743</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="Q3" s="2" t="n">
         <v>2697049</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>54</v>
+        <v>123</v>
       </c>
       <c r="AB3" s="0" t="n">
         <v>0.01</v>
       </c>
       <c r="AC3" s="5" t="n">
         <v>44050</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AG3" s="2" t="n">
+        <v>260236789</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AL3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM3" s="2" t="n">
+        <v>139853010</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AP3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AR3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AS3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AT3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AU3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AV3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AW3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AX3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AY3" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="AZ3" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="BA3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB3" s="2" t="n">
+        <v>503907111</v>
+      </c>
+      <c r="BC3" s="2" t="n">
+        <v>837056</v>
+      </c>
+      <c r="BD3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BE3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BF3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="BG3" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="BH3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="BI3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="BJ3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="BM3" s="0" t="n">
+        <v>350</v>
+      </c>
+      <c r="BN3" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="BO3" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in validation json and in dummy data
</commit_message>
<xml_diff>
--- a/relecov_tools/example_data/dummy_data_small.xlsx
+++ b/relecov_tools/example_data/dummy_data_small.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="132">
   <si>
     <t xml:space="preserve">Collecting Sample id</t>
   </si>
@@ -97,9 +97,6 @@
     <t xml:space="preserve">GISAID Id</t>
   </si>
   <si>
-    <t xml:space="preserve">Originating Laboratory Address</t>
-  </si>
-  <si>
     <t xml:space="preserve">broker_name</t>
   </si>
   <si>
@@ -295,9 +292,6 @@
     <t xml:space="preserve">GISAID-Username</t>
   </si>
   <si>
-    <t xml:space="preserve">Avda. Montevideo,18  BilbaoVizcaya</t>
-  </si>
-  <si>
     <t xml:space="preserve">P17157_1007</t>
   </si>
   <si>
@@ -382,13 +376,19 @@
     <t xml:space="preserve">PRJEB39632</t>
   </si>
   <si>
+    <t xml:space="preserve">asdsa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdsad</t>
+  </si>
+  <si>
     <t xml:space="preserve">PAIRED</t>
   </si>
   <si>
     <t xml:space="preserve">24 degrees celsius</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t xml:space="preserve">covid</t>
   </si>
   <si>
     <t xml:space="preserve">P17157_1008</t>
@@ -407,6 +407,12 @@
   </si>
   <si>
     <t xml:space="preserve">ERX4331407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sadasd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dadsad</t>
   </si>
   <si>
     <t xml:space="preserve">SINGLE</t>
@@ -452,12 +458,24 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFBF00"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -494,9 +512,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -532,6 +558,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFBF00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -540,16 +626,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BP3"/>
+  <dimension ref="A1:BO3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BG1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BP2" activeCellId="0" sqref="BP2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BJ1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BM2" activeCellId="0" sqref="BM2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="0" width="23.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="0" width="23.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1012" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -565,79 +651,79 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="4" t="s">
         <v>21</v>
       </c>
       <c r="W1" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="0" t="s">
         <v>28</v>
       </c>
       <c r="AD1" s="0" t="s">
@@ -646,513 +732,519 @@
       <c r="AE1" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="0" t="s">
+      <c r="AF1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AG1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AH1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AI1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AK1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AL1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AM1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AN1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AO1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AP1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AR1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AS1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AT1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AU1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AV1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AW1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AX1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AY1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BA1" s="0" t="s">
         <v>52</v>
       </c>
       <c r="BB1" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="0" t="s">
+      <c r="BC1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BD1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BE1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BF1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BG1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BH1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BI1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BK1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BL1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BM1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BN1" s="0" t="s">
         <v>65</v>
       </c>
       <c r="BO1" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="0" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="197.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="5" t="n">
+        <v>44743</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="3" t="n">
-        <v>44743</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="Q2" s="4" t="n">
+        <v>2697049</v>
+      </c>
+      <c r="R2" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="Q2" s="2" t="n">
-        <v>2697049</v>
-      </c>
-      <c r="R2" s="0" t="s">
+      <c r="S2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="W2" s="0" t="s">
+      <c r="X2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="Z2" s="0" t="s">
+      <c r="AA2" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AB2" s="7" t="n">
+        <v>44050</v>
+      </c>
+      <c r="AC2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AD2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="AB2" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AC2" s="5" t="n">
-        <v>44050</v>
-      </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="4" t="n">
+        <v>260236789</v>
+      </c>
+      <c r="AG2" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AH2" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="AG2" s="2" t="n">
-        <v>260236789</v>
-      </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AK2" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AL2" s="4" t="n">
+        <v>139853010</v>
+      </c>
+      <c r="AM2" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="AK2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AN2" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="AM2" s="2" t="n">
-        <v>139853010</v>
-      </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AO2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AP2" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AR2" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AS2" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="AS2" s="2" t="s">
+      <c r="AT2" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="AT2" s="2" t="s">
+      <c r="AU2" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="AU2" s="2" t="s">
+      <c r="AV2" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="AV2" s="2" t="s">
+      <c r="AW2" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="AW2" s="2" t="s">
+      <c r="AX2" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="AX2" s="2" t="s">
+      <c r="AY2" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="AY2" s="6" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="AZ2" s="6" t="s">
+      <c r="BA2" s="4" t="n">
+        <v>503907110</v>
+      </c>
+      <c r="BB2" s="4" t="n">
+        <v>837055</v>
+      </c>
+      <c r="BC2" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="BA2" s="2" t="s">
+      <c r="BD2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="BB2" s="2" t="n">
-        <v>503907110</v>
-      </c>
-      <c r="BC2" s="2" t="n">
-        <v>837055</v>
-      </c>
-      <c r="BD2" s="2" t="s">
+      <c r="BE2" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="BF2" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="BE2" s="2" t="s">
+      <c r="BG2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="BF2" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="BG2" s="2" t="s">
+      <c r="BH2" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="BH2" s="2" t="s">
+      <c r="BI2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="BI2" s="2" t="s">
+      <c r="BJ2" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="BJ2" s="2" t="s">
+      <c r="BK2" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="BM2" s="0" t="n">
+      <c r="BL2" s="0" t="n">
         <v>350</v>
       </c>
-      <c r="BN2" s="0" t="s">
+      <c r="BM2" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="BO2" s="2" t="s">
+      <c r="BN2" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="BP2" s="0" t="s">
+      <c r="BO2" s="0" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="197.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="5" t="n">
+        <v>44743</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="3" t="n">
-        <v>44743</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="Q3" s="4" t="n">
+        <v>2697049</v>
+      </c>
+      <c r="R3" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="Q3" s="2" t="n">
-        <v>2697049</v>
-      </c>
-      <c r="R3" s="0" t="s">
+      <c r="S3" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="U3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="W3" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="W3" s="0" t="s">
+      <c r="X3" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="Y3" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="Y3" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z3" s="0" t="s">
+      <c r="Z3" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA3" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AB3" s="7" t="n">
+        <v>44050</v>
+      </c>
+      <c r="AC3" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="AA3" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="AB3" s="0" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AC3" s="5" t="n">
-        <v>44050</v>
-      </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AD3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="AE3" s="2" t="s">
+      <c r="AF3" s="4" t="n">
+        <v>260236789</v>
+      </c>
+      <c r="AG3" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="AF3" s="2" t="s">
+      <c r="AH3" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="AG3" s="2" t="n">
-        <v>260236789</v>
-      </c>
-      <c r="AH3" s="2" t="s">
+      <c r="AI3" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="AI3" s="2" t="s">
+      <c r="AJ3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AK3" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="AJ3" s="2" t="s">
+      <c r="AL3" s="4" t="n">
+        <v>139853010</v>
+      </c>
+      <c r="AM3" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="AK3" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="AL3" s="2" t="s">
+      <c r="AN3" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="AM3" s="2" t="n">
-        <v>139853010</v>
-      </c>
-      <c r="AN3" s="2" t="s">
+      <c r="AO3" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="AO3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AP3" s="2" t="s">
+      <c r="AP3" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="AQ3" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="AQ3" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="AR3" s="2" t="s">
+      <c r="AR3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="AS3" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="AS3" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AT3" s="2" t="s">
+      <c r="AT3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="AU3" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="AU3" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="AV3" s="2" t="s">
+      <c r="AV3" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AW3" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="AW3" s="2" t="s">
+      <c r="AX3" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="AX3" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="AY3" s="6" t="s">
+      <c r="AY3" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="AZ3" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="AZ3" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="BA3" s="2" t="s">
+      <c r="BA3" s="4" t="n">
+        <v>503907111</v>
+      </c>
+      <c r="BB3" s="4" t="n">
+        <v>837056</v>
+      </c>
+      <c r="BC3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="BD3" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="BE3" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="BB3" s="2" t="n">
-        <v>503907111</v>
-      </c>
-      <c r="BC3" s="2" t="n">
-        <v>837056</v>
-      </c>
-      <c r="BD3" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="BE3" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="BF3" s="2" t="s">
+      <c r="BF3" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="BG3" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="BG3" s="2" t="s">
+      <c r="BH3" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="BH3" s="2" t="s">
+      <c r="BI3" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="BI3" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="BJ3" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="BM3" s="0" t="n">
+      <c r="BJ3" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="BK3" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="BL3" s="0" t="n">
         <v>350</v>
       </c>
-      <c r="BN3" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="BO3" s="2" t="s">
+      <c r="BM3" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="BN3" s="4" t="s">
         <v>121</v>
+      </c>
+      <c r="BO3" s="0" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working in json file where fields are already validated and is going to be translated into xml
</commit_message>
<xml_diff>
--- a/relecov_tools/example_data/dummy_data_small.xlsx
+++ b/relecov_tools/example_data/dummy_data_small.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="135">
   <si>
     <t xml:space="preserve">Collecting Sample id</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">Originating Laboratory</t>
   </si>
   <si>
+    <t xml:space="preserve">Originating Laboratory Address</t>
+  </si>
+  <si>
     <t xml:space="preserve">Submitting Institution</t>
   </si>
   <si>
@@ -91,10 +94,10 @@
     <t xml:space="preserve">type</t>
   </si>
   <si>
-    <t xml:space="preserve">GISAID Virus Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GISAID Id</t>
+    <t xml:space="preserve">virus_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">submitter</t>
   </si>
   <si>
     <t xml:space="preserve">broker_name</t>
@@ -229,6 +232,9 @@
     <t xml:space="preserve">Hospital Universitario de Basurto</t>
   </si>
   <si>
+    <t xml:space="preserve">Calle ramon y cajan 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Laboratorio de Microbiología de Bibao </t>
   </si>
   <si>
@@ -289,7 +295,7 @@
     <t xml:space="preserve">hCoV-19/España/Vizcaya-01/2020</t>
   </si>
   <si>
-    <t xml:space="preserve">GISAID-Username</t>
+    <t xml:space="preserve">AS_123</t>
   </si>
   <si>
     <t xml:space="preserve">P17157_1007</t>
@@ -389,6 +395,9 @@
   </si>
   <si>
     <t xml:space="preserve">covid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calle ramon y cajan 3</t>
   </si>
   <si>
     <t xml:space="preserve">P17157_1008</t>
@@ -422,11 +431,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="167" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -541,11 +549,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -626,16 +634,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BO3"/>
+  <dimension ref="A1:BP3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BJ1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BM2" activeCellId="0" sqref="BM2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z4" activeCellId="0" sqref="Z4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="0" width="23.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1012" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1009" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -651,7 +658,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -666,10 +673,10 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
@@ -681,7 +688,7 @@
       <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="4" t="s">
@@ -705,25 +712,25 @@
       <c r="V1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="0" t="s">
         <v>23</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="0" t="s">
         <v>26</v>
       </c>
       <c r="AB1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AC1" s="4" t="s">
         <v>28</v>
       </c>
       <c r="AD1" s="0" t="s">
@@ -732,7 +739,7 @@
       <c r="AE1" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="0" t="s">
         <v>31</v>
       </c>
       <c r="AG1" s="4" t="s">
@@ -795,13 +802,13 @@
       <c r="AZ1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="0" t="s">
+      <c r="BA1" s="4" t="s">
         <v>52</v>
       </c>
       <c r="BB1" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BC1" s="0" t="s">
         <v>54</v>
       </c>
       <c r="BD1" s="4" t="s">
@@ -839,412 +846,421 @@
       </c>
       <c r="BO1" s="0" t="s">
         <v>66</v>
+      </c>
+      <c r="BP1" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="197.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>44743</v>
-      </c>
-      <c r="E2" s="6" t="s">
         <v>70</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>44041</v>
+      </c>
       <c r="F2" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>76</v>
       </c>
+      <c r="K2" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="L2" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="O2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="O2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="Q2" s="4" t="n">
+      <c r="P2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="R2" s="4" t="n">
         <v>2697049</v>
       </c>
-      <c r="R2" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>83</v>
+      <c r="S2" s="0" t="s">
+        <v>84</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="W2" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>88</v>
       </c>
+      <c r="X2" s="0" t="s">
+        <v>89</v>
+      </c>
       <c r="Y2" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA2" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB2" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="AB2" s="7" t="n">
+      <c r="AC2" s="7" t="n">
         <v>44050</v>
       </c>
-      <c r="AC2" s="4" t="s">
-        <v>91</v>
-      </c>
       <c r="AD2" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AE2" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="AF2" s="4" t="n">
+        <v>94</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AG2" s="4" t="n">
         <v>260236789</v>
       </c>
-      <c r="AG2" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="AH2" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AI2" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AJ2" s="4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="AK2" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="AL2" s="4" t="n">
+      <c r="AL2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM2" s="4" t="n">
         <v>139853010</v>
       </c>
-      <c r="AM2" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="AN2" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AO2" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AP2" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AQ2" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AR2" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AS2" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AT2" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AU2" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AV2" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AW2" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="AX2" s="8" t="s">
         <v>109</v>
       </c>
+      <c r="AX2" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="AY2" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="AZ2" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="BA2" s="4" t="n">
+      <c r="AZ2" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="BA2" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB2" s="4" t="n">
         <v>503907110</v>
       </c>
-      <c r="BB2" s="4" t="n">
+      <c r="BC2" s="4" t="n">
         <v>837055</v>
       </c>
-      <c r="BC2" s="4" t="s">
-        <v>112</v>
-      </c>
       <c r="BD2" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="BE2" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="BF2" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="BG2" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="BH2" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="BI2" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="BJ2" s="0" t="s">
         <v>118</v>
       </c>
+      <c r="BJ2" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="BK2" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="BL2" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="BL2" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="BM2" s="0" t="n">
         <v>350</v>
       </c>
-      <c r="BM2" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="BN2" s="4" t="s">
-        <v>121</v>
+      <c r="BN2" s="0" t="s">
+        <v>122</v>
       </c>
       <c r="BO2" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
+      </c>
+      <c r="BP2" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="197.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>44743</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>70</v>
+        <v>125</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>44041</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="G3" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="I3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>76</v>
       </c>
+      <c r="K3" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="L3" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="O3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="O3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="Q3" s="4" t="n">
+      <c r="P3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="R3" s="4" t="n">
         <v>2697049</v>
       </c>
-      <c r="R3" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>83</v>
+      <c r="S3" s="0" t="s">
+        <v>84</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="W3" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="W3" s="4" t="s">
         <v>88</v>
       </c>
+      <c r="X3" s="0" t="s">
+        <v>89</v>
+      </c>
       <c r="Y3" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Z3" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA3" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB3" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="AB3" s="7" t="n">
+      <c r="AC3" s="7" t="n">
         <v>44050</v>
       </c>
-      <c r="AC3" s="4" t="s">
-        <v>91</v>
-      </c>
       <c r="AD3" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AE3" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="AF3" s="4" t="n">
+        <v>94</v>
+      </c>
+      <c r="AF3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AG3" s="4" t="n">
         <v>260236789</v>
       </c>
-      <c r="AG3" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="AH3" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AI3" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AJ3" s="4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="AK3" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="AL3" s="4" t="n">
+      <c r="AL3" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM3" s="4" t="n">
         <v>139853010</v>
       </c>
-      <c r="AM3" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="AN3" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AO3" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AP3" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR3" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AS3" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AT3" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AU3" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="AV3" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AW3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AX3" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AY3" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="AZ3" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="BA3" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB3" s="4" t="n">
+        <v>503907111</v>
+      </c>
+      <c r="BC3" s="4" t="n">
+        <v>837056</v>
+      </c>
+      <c r="BD3" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="BE3" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="BF3" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="BG3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="BH3" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="BI3" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="BJ3" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="BK3" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="BL3" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="BM3" s="0" t="n">
+        <v>350</v>
+      </c>
+      <c r="BN3" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="BO3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="BP3" s="0" t="s">
         <v>124</v>
-      </c>
-      <c r="AQ3" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="AR3" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="AS3" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="AT3" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="AU3" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="AV3" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="AW3" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="AX3" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="AY3" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="AZ3" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="BA3" s="4" t="n">
-        <v>503907111</v>
-      </c>
-      <c r="BB3" s="4" t="n">
-        <v>837056</v>
-      </c>
-      <c r="BC3" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="BD3" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="BE3" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="BF3" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="BG3" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="BH3" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="BI3" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="BJ3" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="BK3" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="BL3" s="0" t="n">
-        <v>350</v>
-      </c>
-      <c r="BM3" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="BN3" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="BO3" s="0" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>